<commit_message>
all excel files added and data added to the database
</commit_message>
<xml_diff>
--- a/sample_excels/grades.xlsx
+++ b/sample_excels/grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\school_onboarding_etl\sample_excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F9545B0-C3C3-45D7-B2B9-291BC4812AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63841457-CAAC-4FDC-B0CD-DDD72B874B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{43BE1E4C-2B8F-4E0F-813F-E373FFF56B47}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{452694CB-E285-403C-8CB0-46ECC48B7980}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>grade_id</t>
+  </si>
   <si>
     <t>school_id</t>
   </si>
@@ -52,16 +55,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -89,11 +84,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,48 +399,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0CA784-6A0A-4FB6-B42D-B40BA30A028B}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1C3F4C-580D-4319-B906-D02913A7B8F6}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>